<commit_message>
Adaptation et type de la fonction create_chart
</commit_message>
<xml_diff>
--- a/gambling.xlsx
+++ b/gambling.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/Desktop/USIDOF/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D45B042-9FEA-C343-888E-FE5713CFE8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="dashboard" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -124,8 +119,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,21 +183,234 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Evolution du nombre d'opérateurs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nombre opérateurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -240,7 +448,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -274,7 +482,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -309,10 +516,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,52 +691,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="34" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="34" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34">
       <c r="A2" s="1">
         <v>2010</v>
       </c>
@@ -714,7 +882,7 @@
         <v>0.08</v>
       </c>
       <c r="AB2">
-        <v>0.81</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AC2">
         <v>0.19</v>
@@ -735,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34">
       <c r="A3" s="1">
         <v>2011</v>
       </c>
@@ -839,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34">
       <c r="A4" s="1">
         <v>2012</v>
       </c>
@@ -922,7 +1090,7 @@
         <v>0.08</v>
       </c>
       <c r="AB4">
-        <v>0.81</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AC4">
         <v>0.19</v>
@@ -943,7 +1111,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34">
       <c r="A5" s="1">
         <v>2013</v>
       </c>
@@ -1011,13 +1179,13 @@
         <v>0.31</v>
       </c>
       <c r="W5">
-        <v>0.69</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="X5">
         <v>0.31</v>
       </c>
       <c r="Y5">
-        <v>0.69</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="Z5">
         <v>0.92</v>
@@ -1026,7 +1194,7 @@
         <v>0.08</v>
       </c>
       <c r="AB5">
-        <v>0.81</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AC5">
         <v>0.19</v>
@@ -1047,7 +1215,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34">
       <c r="A6" s="1">
         <v>2014</v>
       </c>
@@ -1109,7 +1277,7 @@
         <v>0.45</v>
       </c>
       <c r="U6">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="V6">
         <v>0.33</v>
@@ -1127,7 +1295,7 @@
         <v>0.93</v>
       </c>
       <c r="AA6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="AB6">
         <v>0.83</v>
@@ -1151,7 +1319,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -1231,7 +1399,7 @@
         <v>0.93</v>
       </c>
       <c r="AA7">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="AB7">
         <v>0.89</v>
@@ -1246,7 +1414,7 @@
         <v>0.17</v>
       </c>
       <c r="AF7">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="AG7">
         <v>0.2</v>
@@ -1255,7 +1423,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34">
       <c r="A8" s="1">
         <v>2016</v>
       </c>
@@ -1350,7 +1518,7 @@
         <v>0.17</v>
       </c>
       <c r="AF8">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="AG8">
         <v>0.2</v>
@@ -1359,7 +1527,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34">
       <c r="A9" s="1">
         <v>2017</v>
       </c>
@@ -1427,7 +1595,7 @@
         <v>0.44</v>
       </c>
       <c r="W9">
-        <v>0.56000000000000005</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="X9">
         <v>0.51</v>
@@ -1454,7 +1622,7 @@
         <v>0.17</v>
       </c>
       <c r="AF9">
-        <v>0.56999999999999995</v>
+        <v>0.57</v>
       </c>
       <c r="AG9">
         <v>0.21</v>
@@ -1463,7 +1631,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34">
       <c r="A10" s="1">
         <v>2018</v>
       </c>
@@ -1534,7 +1702,7 @@
         <v>0.47</v>
       </c>
       <c r="X10">
-        <v>0.56999999999999995</v>
+        <v>0.57</v>
       </c>
       <c r="Y10">
         <v>0.43</v>
@@ -1567,7 +1735,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34">
       <c r="A11" s="1">
         <v>2019</v>
       </c>
@@ -1632,7 +1800,7 @@
         <v>0.17</v>
       </c>
       <c r="V11">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="W11">
         <v>0.45</v>
@@ -1671,7 +1839,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34">
       <c r="A12" s="1">
         <v>2020</v>
       </c>
@@ -1736,7 +1904,7 @@
         <v>0.1</v>
       </c>
       <c r="V12">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="W12">
         <v>0.42</v>
@@ -1745,7 +1913,7 @@
         <v>0.42</v>
       </c>
       <c r="Y12">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="Z12">
         <v>0.89</v>
@@ -1775,7 +1943,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34">
       <c r="A13" s="1">
         <v>2021</v>
       </c>
@@ -1858,7 +2026,7 @@
         <v>0.15</v>
       </c>
       <c r="AB13">
-        <v>0.81</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AC13">
         <v>0.19</v>
@@ -1879,7 +2047,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34">
       <c r="A14" s="1">
         <v>2022</v>
       </c>
@@ -1959,7 +2127,7 @@
         <v>0.86</v>
       </c>
       <c r="AA14">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AB14">
         <v>0.82</v>
@@ -1974,7 +2142,7 @@
         <v>0.12</v>
       </c>
       <c r="AF14">
-        <v>0.56000000000000005</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AG14">
         <v>0.22</v>
@@ -1986,4 +2154,17 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de mypy pour vérification du typage, Argument size supp dans fonction create_chart, mis à jour du requirement.txt
</commit_message>
<xml_diff>
--- a/gambling.xlsx
+++ b/gambling.xlsx
@@ -336,6 +336,24 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Année</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
@@ -351,6 +369,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nombre d'opérateurs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
@@ -382,10 +418,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>

<commit_message>
Taille des colonnes ajustées
</commit_message>
<xml_diff>
--- a/gambling.xlsx
+++ b/gambling.xlsx
@@ -201,7 +201,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Evolution du nombre d'opérateurs</a:t>
+              <a:t>Évolution du nombre d'opérateurs</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -408,6 +408,228 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Évolution du nombre d'opérateurs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nombre opérateurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Année</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nombre d'opérateurs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -435,6 +657,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -733,6 +985,36 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="45.7109375" customWidth="1"/>
+    <col min="13" max="13" width="43.7109375" customWidth="1"/>
+    <col min="14" max="14" width="46.7109375" customWidth="1"/>
+    <col min="15" max="15" width="44.7109375" customWidth="1"/>
+    <col min="16" max="16" width="46.7109375" customWidth="1"/>
+    <col min="17" max="17" width="61.7109375" customWidth="1"/>
+    <col min="18" max="18" width="34.7109375" customWidth="1"/>
+    <col min="19" max="19" width="48.7109375" customWidth="1"/>
+    <col min="20" max="20" width="46.7109375" customWidth="1"/>
+    <col min="21" max="21" width="32.7109375" customWidth="1"/>
+    <col min="22" max="22" width="46.7109375" customWidth="1"/>
+    <col min="23" max="23" width="32.7109375" customWidth="1"/>
+    <col min="24" max="24" width="46.7109375" customWidth="1"/>
+    <col min="25" max="25" width="32.7109375" customWidth="1"/>
+    <col min="26" max="31" width="22.7109375" customWidth="1"/>
+    <col min="32" max="32" width="24.7109375" customWidth="1"/>
+    <col min="33" max="33" width="22.7109375" customWidth="1"/>
+    <col min="34" max="34" width="26.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34">
       <c r="B1" s="1" t="s">

</xml_diff>